<commit_message>
Finished making assignment 1. Edited guest lectures  a bit
</commit_message>
<xml_diff>
--- a/assignments/assign1/params_assign1.xlsx
+++ b/assignments/assign1/params_assign1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{2C51997A-C534-8C4D-BD22-5FD55DB9965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC7E30F-253B-DE46-95E6-5464A4785BEE}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{2C51997A-C534-8C4D-BD22-5FD55DB9965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3046E919-0396-FF46-8918-E0BF65F44BAE}"/>
   <bookViews>
-    <workbookView xWindow="-37880" yWindow="-580" windowWidth="28380" windowHeight="17500" activeTab="1" xr2:uid="{E22EE68E-8329-254E-8C9B-ADF46AFACE72}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{E22EE68E-8329-254E-8C9B-ADF46AFACE72}"/>
   </bookViews>
   <sheets>
     <sheet name="OTSc" sheetId="1" r:id="rId1"/>
     <sheet name="CEdata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CEdata!$A$1:$E$10</definedName>
     <definedName name="c_hosp_CC">OTSc!$B$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,45 +46,15 @@
     <t>p_ST_rebleed</t>
   </si>
   <si>
-    <t>Continued bleding after an initial EGD using standard therapy</t>
-  </si>
-  <si>
-    <t>p_OTS_rebleed</t>
-  </si>
-  <si>
-    <t>Continued bleding after an initial EGD using OTS clip</t>
-  </si>
-  <si>
     <t>p_ST_rpt_IR</t>
   </si>
   <si>
-    <t>Interventional Radiology (IR) procedure after repeat EGD using standard therapy</t>
-  </si>
-  <si>
-    <t>p_OTS_rpt_IR</t>
-  </si>
-  <si>
-    <t>Interventional Radiology (IR) procedure after repeat  EGD using OTS clip</t>
-  </si>
-  <si>
     <t>c_EGD_MD</t>
   </si>
   <si>
     <t>EGD physician fee (CPT code)</t>
   </si>
   <si>
-    <t>c_Stclip</t>
-  </si>
-  <si>
-    <t>Standard therapy clip</t>
-  </si>
-  <si>
-    <t>c_OTS</t>
-  </si>
-  <si>
-    <t>Over-the-scope clip</t>
-  </si>
-  <si>
     <t>c_hosp_noCC</t>
   </si>
   <si>
@@ -99,33 +70,12 @@
     <t xml:space="preserve">Interventional radiology physician fee </t>
   </si>
   <si>
-    <t>u_EGD</t>
-  </si>
-  <si>
-    <t>Single EGD</t>
-  </si>
-  <si>
-    <t>u_double_EGD</t>
-  </si>
-  <si>
-    <t>Added toll of second EGD</t>
-  </si>
-  <si>
-    <t>u_IR</t>
-  </si>
-  <si>
-    <t>Added toll of IR after two EGDs</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>Utility toll (Quality-adjusted life days lost)</t>
-  </si>
-  <si>
     <t>Hospitalization cost of single successful EGD, based on DRG 379:  GI hemorrhage hospitalization w/o CC</t>
   </si>
   <si>
@@ -193,18 +143,67 @@
   </si>
   <si>
     <t>Cost_productivity</t>
+  </si>
+  <si>
+    <t>p_OTSc_rebleed</t>
+  </si>
+  <si>
+    <t>p_OTSc_rpt_IR</t>
+  </si>
+  <si>
+    <t>Continued bleding after an initial EGD using OTSc</t>
+  </si>
+  <si>
+    <t>Continued bleding after an initial EGD using standard therapy clip</t>
+  </si>
+  <si>
+    <t>Cost of standard therapy clip</t>
+  </si>
+  <si>
+    <t>Cost of over-the-scope clip</t>
+  </si>
+  <si>
+    <t>c_OTSclip</t>
+  </si>
+  <si>
+    <t>c_STclip</t>
+  </si>
+  <si>
+    <t>q_single_EGD</t>
+  </si>
+  <si>
+    <t>q_double_EGD</t>
+  </si>
+  <si>
+    <t>q_IR</t>
+  </si>
+  <si>
+    <t>QALY</t>
+  </si>
+  <si>
+    <t>QALYs experienced in one-year period if single EGD needed (loss of 4.75 quality-adjusted life days)</t>
+  </si>
+  <si>
+    <t>QALYs experienced in one-year period if two EGDs needed (1.1 quality-adjusted life days)</t>
+  </si>
+  <si>
+    <t>QALYs experienced in one-year period if two EGDs and an IR procedure needed (3.65 quality-adjusted life days)</t>
+  </si>
+  <si>
+    <t>Interventional Radiology (IR) procedure needed after second line EGD using standard therapy</t>
+  </si>
+  <si>
+    <t>Interventional Radiology (IR) procedure needed after second line  EGD using OTSc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,13 +228,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,11 +326,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -359,10 +350,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -376,6 +367,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D6BABA-B0B2-9149-BDBF-8E26BBF3268B}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="178" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,35 +686,35 @@
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4">
         <f>0.11</f>
@@ -732,15 +727,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D3" s="6">
         <f>0.053</f>
@@ -753,15 +748,15 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D4" s="8">
         <v>0.57599999999999996</v>
@@ -773,15 +768,15 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D5" s="6">
         <v>0.152</v>
@@ -793,15 +788,15 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D6" s="12">
         <v>192.99</v>
@@ -813,15 +808,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D7" s="15">
         <v>174</v>
@@ -833,15 +828,15 @@
         <v>610</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D8" s="15">
         <v>438</v>
@@ -853,15 +848,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D9" s="15">
         <v>5534.11</v>
@@ -873,15 +868,15 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D10" s="15">
         <v>7503.89</v>
@@ -893,15 +888,15 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D11" s="15">
         <v>13097.08</v>
@@ -913,15 +908,15 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D12" s="15">
         <v>1005.31</v>
@@ -933,70 +928,71 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="12">
-        <v>4.7450000000000001</v>
+        <v>46</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0.98699999999999999</v>
       </c>
       <c r="E13" s="13">
-        <v>0</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="F13" s="13">
-        <f>0.016*365</f>
-        <v>5.84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1.0949999999999998</v>
-      </c>
-      <c r="E14" s="16">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.97</v>
       </c>
       <c r="F14" s="13">
-        <v>4.7450000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="15">
-        <v>3.6500000000000004</v>
-      </c>
-      <c r="E15" s="16">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.93899999999999995</v>
       </c>
       <c r="F15" s="13">
-        <v>18.614999999999998</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H15" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D5">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -1010,7 +1006,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D12">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1032,7 +1028,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{647120B6-5384-AB48-8E30-E12D52A040B0}</x14:id>
+          <x14:id>{50A27838-F519-3C4D-868A-A896032115A1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1072,7 +1068,7 @@
           <xm:sqref>D6:D12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{647120B6-5384-AB48-8E30-E12D52A040B0}">
+          <x14:cfRule type="dataBar" id="{50A27838-F519-3C4D-868A-A896032115A1}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1092,191 +1088,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4DE478-A64C-6B47-8C1D-9F71AB23D39F}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>121</v>
+        <v>1.21</v>
       </c>
       <c r="C2">
-        <v>11000000</v>
+        <v>110000</v>
       </c>
       <c r="D2">
-        <v>108000</v>
+        <v>1080</v>
       </c>
       <c r="E2">
-        <v>131890</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>203</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C3">
-        <v>12000000</v>
+        <v>120000</v>
       </c>
       <c r="D3">
-        <v>1080000</v>
+        <v>10800</v>
       </c>
       <c r="E3">
-        <v>221270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>304</v>
+        <v>3.04</v>
       </c>
       <c r="C4">
-        <v>74700000</v>
+        <v>747000</v>
       </c>
       <c r="D4">
-        <v>22410000</v>
+        <v>224100</v>
       </c>
       <c r="E4">
-        <v>307040</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>343</v>
+        <v>3.43</v>
       </c>
       <c r="C5">
-        <v>50400000</v>
+        <v>504000</v>
       </c>
       <c r="D5">
+        <v>5940</v>
+      </c>
+      <c r="E5">
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>5.03</v>
+      </c>
+      <c r="C6">
+        <v>414000</v>
+      </c>
+      <c r="D6">
+        <v>124200</v>
+      </c>
+      <c r="E6">
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>5.49</v>
+      </c>
+      <c r="C7">
         <v>594000</v>
       </c>
-      <c r="E5">
-        <v>343000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>503</v>
-      </c>
-      <c r="C6">
-        <v>41400000</v>
-      </c>
-      <c r="D6">
-        <v>12420000</v>
-      </c>
-      <c r="E6">
-        <v>482880</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>549</v>
-      </c>
-      <c r="C7">
-        <v>59400000</v>
-      </c>
       <c r="D7">
-        <v>6480000</v>
+        <v>64800</v>
       </c>
       <c r="E7">
-        <v>510570</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>564</v>
+        <v>5.64</v>
       </c>
       <c r="C8">
-        <v>61000000</v>
+        <v>310000</v>
       </c>
       <c r="D8">
-        <v>2376000</v>
+        <v>23760</v>
       </c>
       <c r="E8">
-        <v>541440</v>
-      </c>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>593</v>
+        <v>6.1</v>
       </c>
       <c r="C9">
-        <v>32400000</v>
+        <v>324000</v>
       </c>
       <c r="D9">
-        <v>8100000</v>
+        <v>81000</v>
       </c>
       <c r="E9">
-        <v>539630</v>
-      </c>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>839</v>
+        <v>8.39</v>
       </c>
       <c r="C10">
-        <v>64800000</v>
+        <v>648000</v>
       </c>
       <c r="D10">
-        <v>11088000</v>
+        <v>110880</v>
       </c>
       <c r="E10">
-        <v>864170</v>
+        <v>8641</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E10" xr:uid="{DE4DE478-A64C-6B47-8C1D-9F71AB23D39F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+      <sortCondition ref="B1:B10"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
     <sortCondition ref="B2:B10"/>
   </sortState>

</xml_diff>